<commit_message>
se agrega los indices de la familia MeanSquaredError
</commit_message>
<xml_diff>
--- a/distanciasContinuas.xlsx
+++ b/distanciasContinuas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joseeduardofernandezperez/Google Drive/CIC/TT Eduardo 2017/Codigo/final/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joseeduardofernandezperez/workspace/similitud/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Euclidean</t>
   </si>
@@ -156,6 +156,27 @@
   </si>
   <si>
     <t>JensenDifference</t>
+  </si>
+  <si>
+    <t>MeanSquaredError</t>
+  </si>
+  <si>
+    <t>RootMeanSquaredError</t>
+  </si>
+  <si>
+    <t>MeanAbsoluteError</t>
+  </si>
+  <si>
+    <t>RelativeSquaredError</t>
+  </si>
+  <si>
+    <t>RootRelativeSquaredError</t>
+  </si>
+  <si>
+    <t>RelativeAbsoluteError</t>
+  </si>
+  <si>
+    <t>CorrelationCoefficient</t>
   </si>
 </sst>
 </file>
@@ -470,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A43"/>
+  <dimension ref="A1:A50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -696,6 +717,41 @@
         <v>42</v>
       </c>
     </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>